<commit_message>
added a second approach to estimate the signal loss due to sliding. the Hazard function and survival function where estimated and the report was edited
</commit_message>
<xml_diff>
--- a/Documents/Figure 2C_data.xlsx
+++ b/Documents/Figure 2C_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>UVC</t>
   </si>
@@ -43,6 +43,12 @@
   <si>
     <t>percent lost relative to time 0</t>
   </si>
+  <si>
+    <t>percent lost original</t>
+  </si>
+  <si>
+    <t>percentLost difference</t>
+  </si>
 </sst>
 </file>
 
@@ -51,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -75,16 +81,8 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -95,16 +93,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="22"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -229,33 +224,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>UVC</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -961,7 +933,6 @@
               <a:solidFill>
                 <a:srgbClr val="8064a2"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -1618,11 +1589,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="73917327"/>
-        <c:axId val="15904435"/>
+        <c:axId val="93693212"/>
+        <c:axId val="64848128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73917327"/>
+        <c:axId val="93693212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -1663,11 +1634,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15904435"/>
+        <c:crossAx val="64848128"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15904435"/>
+        <c:axId val="64848128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1708,7 +1679,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73917327"/>
+        <c:crossAx val="93693212"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1717,6 +1688,906 @@
         </a:solidFill>
         <a:ln>
           <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$37:$AZ$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0880148729346994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.176029745869399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.304892463489236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.497887307979186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.634684274739013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.787228986750193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.931461888123447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.09930550451798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.26936852699386</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.40823802336186</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.56458674112244</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.72473236661575</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.86292385226705</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.04528083228843</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1844717416308</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.35511752907464</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.50803789918661</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.65799094985809</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.81096970460208</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.95079632258696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.12917315781407</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.28850720388509</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.44046970145521</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.59031642765422</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.73830136977049</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.91245656281327</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.06014846527988</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.21369841234345</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.37603029008083</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.52571122291575</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.68053877588448</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.84001846890951</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.000608619032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.15920372491154</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.3101504329383</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.46259850167973</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.60814353474329</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.77420588375967</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.93562317869516</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.09276550105793</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.23851030375067</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.39790014104133</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.55341448682794</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.70763316201518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.86967086945307</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.02797374998734</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.18710135290232</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.33644786412772</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.48488572462607</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.65071420990167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$38:$AZ$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>-0.639428479927152</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.634246732253901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.632591903317962</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.61020874622426</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.593171643086589</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.537665436935154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.511077936096932</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.462152912149292</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.405015459728705</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.34696629723686</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.28211355867377</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.205375692269761</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.135743200647792</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00431985990674087</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0881994400416505</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.193390291172456</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.298591295820985</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.491561851267472</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.653259642226878</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.83381838550834</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.996749707103238</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.92127066856542</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.936912261748697</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.846608907969894</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.711033347436593</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.571000687792216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.456847917468643</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.391463202152643</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.336866011710924</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.286650709957508</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.253279718971402</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.255727092224272</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.223156534373569</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.214792264735387</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.191843979938187</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.151709213271111</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.152899033185894</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.139451811916003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.13085606548049</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.123215794500266</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.139851542748564</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.111051365202415</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.130141501687838</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.171552760065517</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.137773348306766</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.173753718356617</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.168664879701939</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.168896563704903</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.153160030438647</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.169206429778361</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="78439248"/>
+        <c:axId val="59391571"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78439248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="2200">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>radius from center</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="59391571"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="59391571"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="2400">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>% gain relative to time 0
+</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="78439248"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ee4000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$37:$AZ$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.0880148729346994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.176029745869399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.304892463489236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.497887307979186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.634684274739013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.787228986750193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.931461888123447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.09930550451798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.26936852699386</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.40823802336186</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.56458674112244</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.72473236661575</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.86292385226705</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.04528083228843</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1844717416308</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.35511752907464</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.50803789918661</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.65799094985809</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.81096970460208</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.95079632258696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.12917315781407</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.28850720388509</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.44046970145521</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.59031642765422</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.73830136977049</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.91245656281327</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.06014846527988</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.21369841234345</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.37603029008083</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.52571122291575</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.68053877588448</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.84001846890951</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.000608619032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.15920372491154</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.3101504329383</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.46259850167973</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.60814353474329</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.77420588375967</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.93562317869516</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.09276550105793</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.23851030375067</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.39790014104133</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.55341448682794</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.70763316201518</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.86967086945307</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.02797374998734</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.18710135290232</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.33644786412772</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.48488572462607</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.65071420990167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$39:$AZ$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>-0.626649040466281</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.628643285936161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.614119376789404</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.591296055607046</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.578620814688087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.524810458684884</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.492301855150109</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.456275044133876</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.421608036091991</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.390603928637084</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.380121044677443</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.373863912501771</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.392609290983521</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.408787013957597</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.451650620911992</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.495650314780596</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.548567756976557</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.601352497435413</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.659274169326757</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.702279407263351</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.75542458371676</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.803656712366919</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.83837808582609</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.863298866786651</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.884226444660059</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.901172490996111</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.91337337388422</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.92144470446843</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.925414641553279</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.929942330978149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.932972771205851</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.934368745063111</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.937300395549511</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.937965910344741</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.939822192551578</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.941567909441219</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.943217161361976</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.944169610049873</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.945177449074352</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.945881337038617</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.94646021246978</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.947381682453831</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.948684221709715</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.94770518595246</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.9488998059924</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.947995850333883</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.948213523816841</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.947880402432676</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.947393617372155</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.94663598611815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="7244592"/>
+        <c:axId val="23604498"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="7244592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="23604498"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="23604498"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="7244592"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -1760,10 +2631,7 @@
               <a:srgbClr val="004586"/>
             </a:solidFill>
             <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
+              <a:noFill/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1936,195 +2804,175 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$C$38:$AZ$38</c:f>
+              <c:f>Feuil1!$C$40:$AZ$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>-0.639428479927152</c:v>
+                  <c:v>-0.662091216981741</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.634246732253901</c:v>
+                  <c:v>-0.643963576448591</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.632591903317962</c:v>
+                  <c:v>-0.664397328460524</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.61020874622426</c:v>
+                  <c:v>-0.639816104310076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.593171643086589</c:v>
+                  <c:v>-0.614387319532777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.537665436935154</c:v>
+                  <c:v>-0.552614951961474</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.511077936096932</c:v>
+                  <c:v>-0.530704869317509</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.462152912149292</c:v>
+                  <c:v>-0.467203555504836</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.405015459728705</c:v>
+                  <c:v>-0.3937206285373</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.34696629723686</c:v>
+                  <c:v>-0.323780989460159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.28211355867377</c:v>
+                  <c:v>-0.24359877546922</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.205375692269761</c:v>
+                  <c:v>-0.161828843107432</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.135743200647792</c:v>
+                  <c:v>-0.095398912623456</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.00431985990674087</c:v>
+                  <c:v>0.00254297199199693</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0881994400416505</c:v>
+                  <c:v>0.044444158306954</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.193390291172456</c:v>
+                  <c:v>0.081730455827231</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.298591295820985</c:v>
+                  <c:v>0.10379997067093</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.491561851267472</c:v>
+                  <c:v>0.131378999937068</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.653259642226878</c:v>
+                  <c:v>0.134632473059857</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.83381838550834</c:v>
+                  <c:v>0.135370495753561</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.996749707103238</c:v>
+                  <c:v>0.122088649207132</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.92127066856542</c:v>
+                  <c:v>0.094148791643774</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.936912261748697</c:v>
+                  <c:v>0.0781788396652108</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.846608907969894</c:v>
+                  <c:v>0.0626729334016008</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.711033347436593</c:v>
+                  <c:v>0.048110610305358</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.571000687792216</c:v>
+                  <c:v>0.0359201469818042</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.456847917468643</c:v>
+                  <c:v>0.0271649451283102</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.391463202152643</c:v>
+                  <c:v>0.0221001227249574</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.336866011710924</c:v>
+                  <c:v>0.0187941588849441</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.286650709957508</c:v>
+                  <c:v>0.0156080281988458</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.253279718971402</c:v>
+                  <c:v>0.0135457690852502</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.255727092224272</c:v>
+                  <c:v>0.0133657146429097</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.223156534373569</c:v>
+                  <c:v>0.0114391135088286</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.214792264735387</c:v>
+                  <c:v>0.0109684947744984</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.191843979938187</c:v>
+                  <c:v>0.0096864608784264</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.151709213271111</c:v>
+                  <c:v>0.0076969832196457</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.152899033185894</c:v>
+                  <c:v>0.0075306170613334</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.139451811916003</c:v>
+                  <c:v>0.0068328023678602</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.13085606548049</c:v>
+                  <c:v>0.0063437457097477</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.123215794500266</c:v>
+                  <c:v>0.0059367701974363</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.139851542748564</c:v>
+                  <c:v>0.0065689448175649</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.111051365202415</c:v>
+                  <c:v>0.0052592851970365</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.130141501687838</c:v>
+                  <c:v>0.00590927103995741</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.171552760065517</c:v>
+                  <c:v>0.0076576318137536</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.137773348306766</c:v>
+                  <c:v>0.0061877392698904</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.173753718356617</c:v>
+                  <c:v>0.0076983052178213</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.168664879701939</c:v>
+                  <c:v>0.0074739644592105</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.168896563704903</c:v>
+                  <c:v>0.0075308810070433</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.153160030438647</c:v>
+                  <c:v>0.0069870572616733</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.169206429778361</c:v>
+                  <c:v>0.0077227887545079</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="27780502"/>
-        <c:axId val="37707008"/>
+        <c:axId val="38790940"/>
+        <c:axId val="6491669"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27780502"/>
+        <c:axId val="38790940"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="2200">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>radius from center</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2135,11 +2983,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37707008"/>
+        <c:crossAx val="6491669"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37707008"/>
+        <c:axId val="6491669"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,27 +3002,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="2400">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>% gain relative to time 0
-</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2185,7 +3012,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27780502"/>
+        <c:crossAx val="38790940"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2197,6 +3024,16 @@
         </a:ln>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:spPr>
@@ -2215,15 +3052,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2097000</xdr:colOff>
+      <xdr:colOff>2124000</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>344160</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2231,8 +3068,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4429800" y="1857600"/>
-        <a:ext cx="7061760" cy="4495320"/>
+        <a:off x="4456800" y="1848600"/>
+        <a:ext cx="11832480" cy="4494960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2245,15 +3082,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>748800</xdr:colOff>
+      <xdr:colOff>775800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1013400</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>16560</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2261,12 +3098,72 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3081600" y="7967520"/>
-        <a:ext cx="12150000" cy="4112640"/>
+        <a:off x="3108600" y="7958520"/>
+        <a:ext cx="12149640" cy="4112280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1012680</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>179280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>622440</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>179640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="17278200" y="8180280"/>
+        <a:ext cx="5751360" cy="3238560"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>815760</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>67320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>425160</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>67320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8892000" y="12830760"/>
+        <a:ext cx="5751360" cy="3238560"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2280,10 +3177,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AZ38"/>
+  <dimension ref="A1:AZ40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR25" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BE38" activeCellId="0" sqref="BE38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BA69" activeCellId="0" sqref="BA69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3797,6 +4694,416 @@
         <v>0.169206429778361</v>
       </c>
     </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">C3-1</f>
+        <v>-0.626649040466281</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">D3-1</f>
+        <v>-0.628643285936161</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">E3-1</f>
+        <v>-0.614119376789404</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">F3-1</f>
+        <v>-0.591296055607046</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">G3-1</f>
+        <v>-0.578620814688087</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">H3-1</f>
+        <v>-0.524810458684884</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <f aca="false">I3-1</f>
+        <v>-0.492301855150109</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <f aca="false">J3-1</f>
+        <v>-0.456275044133876</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <f aca="false">K3-1</f>
+        <v>-0.421608036091991</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <f aca="false">L3-1</f>
+        <v>-0.390603928637084</v>
+      </c>
+      <c r="M39" s="0" t="n">
+        <f aca="false">M3-1</f>
+        <v>-0.380121044677443</v>
+      </c>
+      <c r="N39" s="0" t="n">
+        <f aca="false">N3-1</f>
+        <v>-0.373863912501771</v>
+      </c>
+      <c r="O39" s="0" t="n">
+        <f aca="false">O3-1</f>
+        <v>-0.392609290983521</v>
+      </c>
+      <c r="P39" s="0" t="n">
+        <f aca="false">P3-1</f>
+        <v>-0.408787013957597</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <f aca="false">Q3-1</f>
+        <v>-0.451650620911992</v>
+      </c>
+      <c r="R39" s="0" t="n">
+        <f aca="false">R3-1</f>
+        <v>-0.495650314780596</v>
+      </c>
+      <c r="S39" s="0" t="n">
+        <f aca="false">S3-1</f>
+        <v>-0.548567756976557</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <f aca="false">T3-1</f>
+        <v>-0.601352497435413</v>
+      </c>
+      <c r="U39" s="0" t="n">
+        <f aca="false">U3-1</f>
+        <v>-0.659274169326757</v>
+      </c>
+      <c r="V39" s="0" t="n">
+        <f aca="false">V3-1</f>
+        <v>-0.702279407263351</v>
+      </c>
+      <c r="W39" s="0" t="n">
+        <f aca="false">W3-1</f>
+        <v>-0.75542458371676</v>
+      </c>
+      <c r="X39" s="0" t="n">
+        <f aca="false">X3-1</f>
+        <v>-0.803656712366919</v>
+      </c>
+      <c r="Y39" s="0" t="n">
+        <f aca="false">Y3-1</f>
+        <v>-0.83837808582609</v>
+      </c>
+      <c r="Z39" s="0" t="n">
+        <f aca="false">Z3-1</f>
+        <v>-0.863298866786651</v>
+      </c>
+      <c r="AA39" s="0" t="n">
+        <f aca="false">AA3-1</f>
+        <v>-0.884226444660059</v>
+      </c>
+      <c r="AB39" s="0" t="n">
+        <f aca="false">AB3-1</f>
+        <v>-0.901172490996111</v>
+      </c>
+      <c r="AC39" s="0" t="n">
+        <f aca="false">AC3-1</f>
+        <v>-0.91337337388422</v>
+      </c>
+      <c r="AD39" s="0" t="n">
+        <f aca="false">AD3-1</f>
+        <v>-0.92144470446843</v>
+      </c>
+      <c r="AE39" s="0" t="n">
+        <f aca="false">AE3-1</f>
+        <v>-0.925414641553279</v>
+      </c>
+      <c r="AF39" s="0" t="n">
+        <f aca="false">AF3-1</f>
+        <v>-0.929942330978149</v>
+      </c>
+      <c r="AG39" s="0" t="n">
+        <f aca="false">AG3-1</f>
+        <v>-0.932972771205851</v>
+      </c>
+      <c r="AH39" s="0" t="n">
+        <f aca="false">AH3-1</f>
+        <v>-0.934368745063111</v>
+      </c>
+      <c r="AI39" s="0" t="n">
+        <f aca="false">AI3-1</f>
+        <v>-0.937300395549511</v>
+      </c>
+      <c r="AJ39" s="0" t="n">
+        <f aca="false">AJ3-1</f>
+        <v>-0.937965910344741</v>
+      </c>
+      <c r="AK39" s="0" t="n">
+        <f aca="false">AK3-1</f>
+        <v>-0.939822192551578</v>
+      </c>
+      <c r="AL39" s="0" t="n">
+        <f aca="false">AL3-1</f>
+        <v>-0.941567909441219</v>
+      </c>
+      <c r="AM39" s="0" t="n">
+        <f aca="false">AM3-1</f>
+        <v>-0.943217161361976</v>
+      </c>
+      <c r="AN39" s="0" t="n">
+        <f aca="false">AN3-1</f>
+        <v>-0.944169610049873</v>
+      </c>
+      <c r="AO39" s="0" t="n">
+        <f aca="false">AO3-1</f>
+        <v>-0.945177449074352</v>
+      </c>
+      <c r="AP39" s="0" t="n">
+        <f aca="false">AP3-1</f>
+        <v>-0.945881337038617</v>
+      </c>
+      <c r="AQ39" s="0" t="n">
+        <f aca="false">AQ3-1</f>
+        <v>-0.94646021246978</v>
+      </c>
+      <c r="AR39" s="0" t="n">
+        <f aca="false">AR3-1</f>
+        <v>-0.947381682453831</v>
+      </c>
+      <c r="AS39" s="0" t="n">
+        <f aca="false">AS3-1</f>
+        <v>-0.948684221709715</v>
+      </c>
+      <c r="AT39" s="0" t="n">
+        <f aca="false">AT3-1</f>
+        <v>-0.94770518595246</v>
+      </c>
+      <c r="AU39" s="0" t="n">
+        <f aca="false">AU3-1</f>
+        <v>-0.9488998059924</v>
+      </c>
+      <c r="AV39" s="0" t="n">
+        <f aca="false">AV3-1</f>
+        <v>-0.947995850333883</v>
+      </c>
+      <c r="AW39" s="0" t="n">
+        <f aca="false">AW3-1</f>
+        <v>-0.948213523816841</v>
+      </c>
+      <c r="AX39" s="0" t="n">
+        <f aca="false">AX3-1</f>
+        <v>-0.947880402432676</v>
+      </c>
+      <c r="AY39" s="0" t="n">
+        <f aca="false">AY3-1</f>
+        <v>-0.947393617372155</v>
+      </c>
+      <c r="AZ39" s="0" t="n">
+        <f aca="false">AZ3-1</f>
+        <v>-0.94663598611815</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">C3-C4</f>
+        <v>-0.662091216981741</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">D3-D4</f>
+        <v>-0.643963576448591</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">E3-E4</f>
+        <v>-0.664397328460524</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">F3-F4</f>
+        <v>-0.639816104310076</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">G3-G4</f>
+        <v>-0.614387319532777</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">H3-H4</f>
+        <v>-0.552614951961474</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <f aca="false">I3-I4</f>
+        <v>-0.530704869317509</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <f aca="false">J3-J4</f>
+        <v>-0.467203555504836</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <f aca="false">K3-K4</f>
+        <v>-0.3937206285373</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <f aca="false">L3-L4</f>
+        <v>-0.323780989460159</v>
+      </c>
+      <c r="M40" s="0" t="n">
+        <f aca="false">M3-M4</f>
+        <v>-0.24359877546922</v>
+      </c>
+      <c r="N40" s="0" t="n">
+        <f aca="false">N3-N4</f>
+        <v>-0.161828843107432</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <f aca="false">O3-O4</f>
+        <v>-0.095398912623456</v>
+      </c>
+      <c r="P40" s="0" t="n">
+        <f aca="false">P3-P4</f>
+        <v>0.00254297199199693</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <f aca="false">Q3-Q4</f>
+        <v>0.044444158306954</v>
+      </c>
+      <c r="R40" s="0" t="n">
+        <f aca="false">R3-R4</f>
+        <v>0.081730455827231</v>
+      </c>
+      <c r="S40" s="0" t="n">
+        <f aca="false">S3-S4</f>
+        <v>0.10379997067093</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <f aca="false">T3-T4</f>
+        <v>0.131378999937068</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <f aca="false">U3-U4</f>
+        <v>0.134632473059857</v>
+      </c>
+      <c r="V40" s="0" t="n">
+        <f aca="false">V3-V4</f>
+        <v>0.135370495753561</v>
+      </c>
+      <c r="W40" s="0" t="n">
+        <f aca="false">W3-W4</f>
+        <v>0.122088649207132</v>
+      </c>
+      <c r="X40" s="0" t="n">
+        <f aca="false">X3-X4</f>
+        <v>0.094148791643774</v>
+      </c>
+      <c r="Y40" s="0" t="n">
+        <f aca="false">Y3-Y4</f>
+        <v>0.0781788396652108</v>
+      </c>
+      <c r="Z40" s="0" t="n">
+        <f aca="false">Z3-Z4</f>
+        <v>0.0626729334016008</v>
+      </c>
+      <c r="AA40" s="0" t="n">
+        <f aca="false">AA3-AA4</f>
+        <v>0.048110610305358</v>
+      </c>
+      <c r="AB40" s="0" t="n">
+        <f aca="false">AB3-AB4</f>
+        <v>0.0359201469818042</v>
+      </c>
+      <c r="AC40" s="0" t="n">
+        <f aca="false">AC3-AC4</f>
+        <v>0.0271649451283102</v>
+      </c>
+      <c r="AD40" s="0" t="n">
+        <f aca="false">AD3-AD4</f>
+        <v>0.0221001227249574</v>
+      </c>
+      <c r="AE40" s="0" t="n">
+        <f aca="false">AE3-AE4</f>
+        <v>0.0187941588849441</v>
+      </c>
+      <c r="AF40" s="0" t="n">
+        <f aca="false">AF3-AF4</f>
+        <v>0.0156080281988458</v>
+      </c>
+      <c r="AG40" s="0" t="n">
+        <f aca="false">AG3-AG4</f>
+        <v>0.0135457690852502</v>
+      </c>
+      <c r="AH40" s="0" t="n">
+        <f aca="false">AH3-AH4</f>
+        <v>0.0133657146429097</v>
+      </c>
+      <c r="AI40" s="0" t="n">
+        <f aca="false">AI3-AI4</f>
+        <v>0.0114391135088286</v>
+      </c>
+      <c r="AJ40" s="0" t="n">
+        <f aca="false">AJ3-AJ4</f>
+        <v>0.0109684947744984</v>
+      </c>
+      <c r="AK40" s="0" t="n">
+        <f aca="false">AK3-AK4</f>
+        <v>0.0096864608784264</v>
+      </c>
+      <c r="AL40" s="0" t="n">
+        <f aca="false">AL3-AL4</f>
+        <v>0.0076969832196457</v>
+      </c>
+      <c r="AM40" s="0" t="n">
+        <f aca="false">AM3-AM4</f>
+        <v>0.0075306170613334</v>
+      </c>
+      <c r="AN40" s="0" t="n">
+        <f aca="false">AN3-AN4</f>
+        <v>0.0068328023678602</v>
+      </c>
+      <c r="AO40" s="0" t="n">
+        <f aca="false">AO3-AO4</f>
+        <v>0.0063437457097477</v>
+      </c>
+      <c r="AP40" s="0" t="n">
+        <f aca="false">AP3-AP4</f>
+        <v>0.0059367701974363</v>
+      </c>
+      <c r="AQ40" s="0" t="n">
+        <f aca="false">AQ3-AQ4</f>
+        <v>0.0065689448175649</v>
+      </c>
+      <c r="AR40" s="0" t="n">
+        <f aca="false">AR3-AR4</f>
+        <v>0.0052592851970365</v>
+      </c>
+      <c r="AS40" s="0" t="n">
+        <f aca="false">AS3-AS4</f>
+        <v>0.00590927103995741</v>
+      </c>
+      <c r="AT40" s="0" t="n">
+        <f aca="false">AT3-AT4</f>
+        <v>0.0076576318137536</v>
+      </c>
+      <c r="AU40" s="0" t="n">
+        <f aca="false">AU3-AU4</f>
+        <v>0.0061877392698904</v>
+      </c>
+      <c r="AV40" s="0" t="n">
+        <f aca="false">AV3-AV4</f>
+        <v>0.0076983052178213</v>
+      </c>
+      <c r="AW40" s="0" t="n">
+        <f aca="false">AW3-AW4</f>
+        <v>0.0074739644592105</v>
+      </c>
+      <c r="AX40" s="0" t="n">
+        <f aca="false">AX3-AX4</f>
+        <v>0.0075308810070433</v>
+      </c>
+      <c r="AY40" s="0" t="n">
+        <f aca="false">AY3-AY4</f>
+        <v>0.0069870572616733</v>
+      </c>
+      <c r="AZ40" s="0" t="n">
+        <f aca="false">AZ3-AZ4</f>
+        <v>0.0077227887545079</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>